<commit_message>
100 unrelated subj for schaefer
</commit_message>
<xml_diff>
--- a/results/effects.xlsx
+++ b/results/effects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Google Drive/Code/fmri_learning/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{586A078C-4766-8E43-993C-4108F28AF100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FEB83A-31A1-0144-B8A3-6104855B73AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1980" yWindow="2460" windowWidth="26440" windowHeight="15040" xr2:uid="{6ABBD25E-18ED-0F49-8978-AAB30722C93C}"/>
   </bookViews>
@@ -32,12 +32,41 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Tangent</t>
+  </si>
+  <si>
+    <t>PCA</t>
+  </si>
+  <si>
+    <t>Raw</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -51,7 +80,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -59,12 +88,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,12 +419,506 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6109723E-2922-D847-98BA-1981EA1F114E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>0.99671052599999999</v>
+      </c>
+      <c r="B2">
+        <v>0.95357406</v>
+      </c>
+      <c r="C2">
+        <v>0.953574060427413</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>0.99342105300000005</v>
+      </c>
+      <c r="B3">
+        <v>0.95799557999999996</v>
+      </c>
+      <c r="C3">
+        <v>0.95210022107590198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>0.98026315799999997</v>
+      </c>
+      <c r="B4">
+        <v>0.95431098000000003</v>
+      </c>
+      <c r="C4">
+        <v>0.94399410464259303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>0.98684210500000002</v>
+      </c>
+      <c r="B5">
+        <v>0.95652174000000001</v>
+      </c>
+      <c r="C5">
+        <v>0.94620486366986001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>0.98684210500000002</v>
+      </c>
+      <c r="B6">
+        <v>0.95873249999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.94915254237288105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>0.98684210500000002</v>
+      </c>
+      <c r="B7">
+        <v>0.95652174000000001</v>
+      </c>
+      <c r="C7">
+        <v>0.95652173913043403</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>0.98026315799999997</v>
+      </c>
+      <c r="B8">
+        <v>0.95725866000000004</v>
+      </c>
+      <c r="C8">
+        <v>0.94767870302137003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>0.96020634000000005</v>
+      </c>
+      <c r="C9">
+        <v>0.94841562269712598</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>0.99671052599999999</v>
+      </c>
+      <c r="B10">
+        <v>0.95283713999999997</v>
+      </c>
+      <c r="C10">
+        <v>0.94473102431834899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>0.98684210500000002</v>
+      </c>
+      <c r="B11">
+        <v>0.95578481999999998</v>
+      </c>
+      <c r="C11">
+        <v>0.95652173913043403</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>0.98684210500000002</v>
+      </c>
+      <c r="B12">
+        <v>0.96094325999999997</v>
+      </c>
+      <c r="C12">
+        <v>0.94915254237288105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>0.96020634000000005</v>
+      </c>
+      <c r="C13">
+        <v>0.94841562269712598</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>0.99671052599999999</v>
+      </c>
+      <c r="B14">
+        <v>0.95799557999999996</v>
+      </c>
+      <c r="C14">
+        <v>0.93957258658806098</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>0.98026315799999997</v>
+      </c>
+      <c r="B15">
+        <v>0.95799557999999996</v>
+      </c>
+      <c r="C15">
+        <v>0.95504789977892401</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>0.98684210500000002</v>
+      </c>
+      <c r="B16">
+        <v>0.95725866000000004</v>
+      </c>
+      <c r="C16">
+        <v>0.95283714075165804</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>0.99671052599999999</v>
+      </c>
+      <c r="B17">
+        <v>0.95578481999999998</v>
+      </c>
+      <c r="C17">
+        <v>0.94620486366986001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>0.95725866000000004</v>
+      </c>
+      <c r="C18">
+        <v>0.95210022107590198</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>0.99671052599999999</v>
+      </c>
+      <c r="B19">
+        <v>0.95873249999999999</v>
+      </c>
+      <c r="C19">
+        <v>0.94841562269712598</v>
+      </c>
+      <c r="E19">
+        <f>AVERAGE(A2:C21)</f>
+        <v>0.96583662228646527</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>0.95136330000000002</v>
+      </c>
+      <c r="C20">
+        <v>0.94473102431834899</v>
+      </c>
+      <c r="E20">
+        <f>AVERAGE(A21:C41)</f>
+        <v>0.94458963849816957</v>
+      </c>
+      <c r="F20">
+        <f>E19-E20</f>
+        <v>2.1246983788295704E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>0.98684210500000002</v>
+      </c>
+      <c r="B21">
+        <v>0.95504789999999995</v>
+      </c>
+      <c r="C21">
+        <v>0.95283714075165804</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>0.98684210500000002</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.94325718000000003</v>
+      </c>
+      <c r="C22">
+        <v>0.90346352247605</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>0.98684210500000002</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.93957259000000004</v>
+      </c>
+      <c r="C23">
+        <v>0.91009579955784803</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>0.98099095999999997</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.94399409999999995</v>
+      </c>
+      <c r="C24">
+        <v>0.91083271923360298</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>0.98684210500000002</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.94325718000000003</v>
+      </c>
+      <c r="C25">
+        <v>0.89904200442151805</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>0.98684210500000002</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.94325718000000003</v>
+      </c>
+      <c r="C26">
+        <v>0.90714812085482599</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>0.98684210500000002</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.94178335000000002</v>
+      </c>
+      <c r="C27">
+        <v>0.89830508474576198</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>0.98026315799999997</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.93883567000000001</v>
+      </c>
+      <c r="C28">
+        <v>0.89683124539425196</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>0.98099095999999997</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.93588799</v>
+      </c>
+      <c r="C29">
+        <v>0.88946204863669798</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <v>0.98684210500000002</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.93367723000000002</v>
+      </c>
+      <c r="C30">
+        <v>0.89904200442151805</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <v>0.98684210500000002</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.94252027000000005</v>
+      </c>
+      <c r="C31">
+        <v>0.90567428150331597</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>0.98684210500000002</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.93957259000000004</v>
+      </c>
+      <c r="C32">
+        <v>0.91083271923360298</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>0.98026315799999997</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.93588799</v>
+      </c>
+      <c r="C33">
+        <v>0.91893883566691204</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>0.98684210500000002</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.94178335000000002</v>
+      </c>
+      <c r="C34">
+        <v>0.90198968312453898</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>0.98026315799999997</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.94252027000000005</v>
+      </c>
+      <c r="C35">
+        <v>0.899778924097273</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>0.98684210500000002</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.94399409999999995</v>
+      </c>
+      <c r="C36">
+        <v>0.90714812085482599</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>0.99671052599999999</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.94030950999999996</v>
+      </c>
+      <c r="C37">
+        <v>0.92114959469417801</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>0.98026315799999997</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.94030950999999996</v>
+      </c>
+      <c r="C38">
+        <v>0.90788504053058205</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>0.98684210500000002</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.93515106999999997</v>
+      </c>
+      <c r="C39">
+        <v>0.90346352247605</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>0.98026315799999997</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.93957259000000004</v>
+      </c>
+      <c r="C40">
+        <v>0.91378039793662402</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>0.98684210500000002</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.94178335000000002</v>
+      </c>
+      <c r="C41">
+        <v>0.90051584377302796</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="2">
+        <f>AVERAGE(A2:A41)</f>
+        <v>0.98819428470000026</v>
+      </c>
+      <c r="B42" s="2">
+        <f t="shared" ref="B42:C42" si="0">AVERAGE(B2:B41)</f>
+        <v>0.94858143075000023</v>
+      </c>
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>0.92733971997052289</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <f>A42-C42</f>
+        <v>6.0854564729477367E-2</v>
+      </c>
+      <c r="B43">
+        <f>B42-C42</f>
+        <v>2.1241710779477341E-2</v>
+      </c>
+      <c r="C43">
+        <f>C42-C42</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>